<commit_message>
Save files to output
</commit_message>
<xml_diff>
--- a/search_result.xlsx
+++ b/search_result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>output\images\29sp-bahrain-preview-inyt-gwpc-threeByTwoSmallAt2X.png</t>
+          <t>output\29sp-bahrain-preview-inyt-gwpc-threeByTwoSmallAt2X.png</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -511,7 +511,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>output\images\29sp-bahrain-haas-inyt-01-qblp-threeByTwoSmallAt2X.png</t>
+          <t>output\29sp-bahrain-haas-inyt-01-qblp-threeByTwoSmallAt2X.png</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -539,7 +539,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>output\images\29sp-bahrain-names-inyt-02-zwbv-threeByTwoSmallAt2X.png</t>
+          <t>output\29sp-bahrain-names-inyt-02-zwbv-threeByTwoSmallAt2X.png</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -567,7 +567,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>output\images\13sp-australian-changes-inyt-01-twbg-threeByTwoSmallAt2X.png</t>
+          <t>output\13sp-australian-changes-inyt-01-twbg-threeByTwoSmallAt2X.png</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -595,7 +595,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>output\images\14sp-review-redbull-inyt-01-jzbh-threeByTwoSmallAt2X.png</t>
+          <t>output\14sp-review-redbull-inyt-01-jzbh-threeByTwoSmallAt2X.png</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -623,7 +623,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>output\images\14sp-review-cars-inyt-02-wkvz-threeByTwoSmallAt2X.png</t>
+          <t>output\14sp-review-cars-inyt-02-wkvz-threeByTwoSmallAt2X.png</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -651,7 +651,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>output\images\14sp-review-aston-inyt-05-mftl-threeByTwoSmallAt2X.png</t>
+          <t>output\14sp-review-aston-inyt-05-mftl-threeByTwoSmallAt2X.png</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -679,7 +679,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>output\images\14sp-review-teams-inyt-02-ghmz-threeByTwoSmallAt2X.png</t>
+          <t>output\14sp-review-teams-inyt-02-ghmz-threeByTwoSmallAt2X.png</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -707,7 +707,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>output\images\14sp-review-tost-inyt-thlv-threeByTwoSmallAt2X.png</t>
+          <t>output\14sp-review-tost-inyt-thlv-threeByTwoSmallAt2X.png</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -735,13 +735,125 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>output\images\09sp-year-roundup-inyt-01-fcwt-threeByTwoSmallAt2X.png</t>
+          <t>output\09sp-year-roundup-inyt-01-fcwt-threeByTwoSmallAt2X.png</t>
         </is>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Gianpiero Lambiase Is the Man in Max Verstappen’s Ear</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Nov. 23, 2023</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>The race engineer gives advice to the driver on the radio during races. Their relationship has been described as a long marriage.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>output\25sp-dhabi-lambiase-inyt-02-hvqf-threeByTwoSmallAt2X.png</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>On Second Thought, Haas Is Staying Put</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Nov. 23, 2023</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Gene Haas once considered selling the team, but changes in F1 have convinced him not to.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>output\25sp-dhabi-haas-inyt-01-wphb-threeByTwoSmallAt2X.png</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>McLaren Is No Longer Caught in the Middle of Formula 1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Nov. 23, 2023</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>The team started the year as another lackluster midfield team, but big changes have moved it to No. 4.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>output\25sp-dhabi-mclaren-inyt-01-hlcq-threeByTwoSmallAt2X.png</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>The Power and Speed of Jannik Sinner</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Nov. 10, 2023</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Sinner, 22, has dominating talent and has already beaten many of tennis’s top players.</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>output\11sp-atp-sinner-inyt3-glvf-threeByTwoSmallAt2X.png</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>